<commit_message>
pushing what I currently have before making big changes
</commit_message>
<xml_diff>
--- a/prep/02_feed/diet_composition_wrangling/salmon_aquaculture_diet_composition.xlsx
+++ b/prep/02_feed/diet_composition_wrangling/salmon_aquaculture_diet_composition.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10" conformance="strict">
+<workbook xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2" conformance="strict">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11012"/>
   <workbookPr dateCompatibility="0" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gclawson/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1EEE09EA-796B-A144-9229-82EB400F0207}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{D68ED266-4730-9847-A74D-485029FF4E9C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4300" yWindow="2700" windowWidth="27640" windowHeight="16940" activeTab="1"/>
+    <workbookView xWindow="-36900" yWindow="1300" windowWidth="27640" windowHeight="16940" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2016" sheetId="1" r:id="rId1"/>
     <sheet name="2020" sheetId="2" r:id="rId2"/>
+    <sheet name="fish-dominant" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="122" uniqueCount="38">
+<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="189" uniqueCount="39">
   <si>
     <t>species</t>
   </si>
@@ -140,12 +141,15 @@
   </si>
   <si>
     <t>other</t>
+  </si>
+  <si>
+    <t xml:space="preserve">soybean meal </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18">
     <font>
       <sz val="12"/>
@@ -979,7 +983,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1265,11 +1269,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C22" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1575,4 +1579,292 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4954F1F7-25CD-4C45-BDC1-E6036E057A74}">
+  <dimension ref="A1:D22"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <cols>
+    <col min="2" max="2" width="16.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3">
+        <v>13</v>
+      </c>
+      <c r="D3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7">
+        <v>4</v>
+      </c>
+      <c r="D7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8" t="s">
+        <v>5</v>
+      </c>
+      <c r="D8" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" t="s">
+        <v>4</v>
+      </c>
+      <c r="B9" t="s">
+        <v>5</v>
+      </c>
+      <c r="D9" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" t="s">
+        <v>4</v>
+      </c>
+      <c r="B10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D10" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" t="s">
+        <v>4</v>
+      </c>
+      <c r="B11" t="s">
+        <v>5</v>
+      </c>
+      <c r="D11" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" t="s">
+        <v>4</v>
+      </c>
+      <c r="B12" t="s">
+        <v>5</v>
+      </c>
+      <c r="D12" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" t="s">
+        <v>4</v>
+      </c>
+      <c r="B13" t="s">
+        <v>5</v>
+      </c>
+      <c r="C13">
+        <v>7</v>
+      </c>
+      <c r="D13" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" t="s">
+        <v>4</v>
+      </c>
+      <c r="B14" t="s">
+        <v>5</v>
+      </c>
+      <c r="C14">
+        <v>2</v>
+      </c>
+      <c r="D14" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" t="s">
+        <v>4</v>
+      </c>
+      <c r="B15" t="s">
+        <v>5</v>
+      </c>
+      <c r="D15" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16" t="s">
+        <v>4</v>
+      </c>
+      <c r="B16" t="s">
+        <v>5</v>
+      </c>
+      <c r="C16">
+        <v>32</v>
+      </c>
+      <c r="D16" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" t="s">
+        <v>4</v>
+      </c>
+      <c r="B17" t="s">
+        <v>5</v>
+      </c>
+      <c r="D17" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18" t="s">
+        <v>4</v>
+      </c>
+      <c r="B18" t="s">
+        <v>5</v>
+      </c>
+      <c r="C18">
+        <v>23</v>
+      </c>
+      <c r="D18" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19" t="s">
+        <v>4</v>
+      </c>
+      <c r="B19" t="s">
+        <v>5</v>
+      </c>
+      <c r="D19" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
+      <c r="A20" t="s">
+        <v>4</v>
+      </c>
+      <c r="B20" t="s">
+        <v>5</v>
+      </c>
+      <c r="C20">
+        <v>2</v>
+      </c>
+      <c r="D20" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
+      <c r="A21" t="s">
+        <v>4</v>
+      </c>
+      <c r="B21" t="s">
+        <v>5</v>
+      </c>
+      <c r="D21" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4">
+      <c r="A22" t="s">
+        <v>4</v>
+      </c>
+      <c r="B22" t="s">
+        <v>5</v>
+      </c>
+      <c r="C22">
+        <v>17</v>
+      </c>
+      <c r="D22" t="s">
+        <v>38</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
figured out mass allocation for crops
</commit_message>
<xml_diff>
--- a/prep/02_feed/diet_composition_wrangling/salmon_aquaculture_diet_composition.xlsx
+++ b/prep/02_feed/diet_composition_wrangling/salmon_aquaculture_diet_composition.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gclawson/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D68ED266-4730-9847-A74D-485029FF4E9C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{F9AEFBF3-E142-7F47-9FAF-C3072D092F02}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-36900" yWindow="1300" windowWidth="27640" windowHeight="16940" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="189" uniqueCount="39">
+<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="232" uniqueCount="44">
   <si>
     <t>species</t>
   </si>
@@ -144,6 +144,21 @@
   </si>
   <si>
     <t xml:space="preserve">soybean meal </t>
+  </si>
+  <si>
+    <t>raw_name_edit</t>
+  </si>
+  <si>
+    <t>guar meal</t>
+  </si>
+  <si>
+    <t>corn gluten meal</t>
+  </si>
+  <si>
+    <t>canola oil</t>
+  </si>
+  <si>
+    <t>soy oil</t>
   </si>
 </sst>
 </file>
@@ -1270,19 +1285,20 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:D21"/>
+  <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C22" sqref="A1:XFD1048576"/>
+      <selection activeCell="E16" sqref="E16:E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="2" max="2" width="16.83203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="20.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1295,8 +1311,11 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4">
+      <c r="E1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -1309,8 +1328,11 @@
       <c r="D2" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="3" spans="1:4">
+      <c r="E2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -1323,8 +1345,11 @@
       <c r="D3" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="4" spans="1:4">
+      <c r="E3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -1337,8 +1362,11 @@
       <c r="D4" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="5" spans="1:4">
+      <c r="E4" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -1351,8 +1379,11 @@
       <c r="D5" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="6" spans="1:4">
+      <c r="E5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -1365,8 +1396,11 @@
       <c r="D6" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="7" spans="1:4">
+      <c r="E6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -1379,8 +1413,11 @@
       <c r="D7" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="8" spans="1:4">
+      <c r="E7" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
       <c r="A8" t="s">
         <v>4</v>
       </c>
@@ -1393,8 +1430,11 @@
       <c r="D8" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="9" spans="1:4">
+      <c r="E8" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
       <c r="A9" t="s">
         <v>4</v>
       </c>
@@ -1407,8 +1447,11 @@
       <c r="D9" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="10" spans="1:4">
+      <c r="E9" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
       <c r="A10" t="s">
         <v>4</v>
       </c>
@@ -1421,8 +1464,11 @@
       <c r="D10" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="11" spans="1:4">
+      <c r="E10" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
       <c r="A11" t="s">
         <v>4</v>
       </c>
@@ -1435,8 +1481,11 @@
       <c r="D11" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="12" spans="1:4">
+      <c r="E11" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
       <c r="A12" t="s">
         <v>4</v>
       </c>
@@ -1449,8 +1498,11 @@
       <c r="D12" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="13" spans="1:4">
+      <c r="E12" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
       <c r="A13" t="s">
         <v>4</v>
       </c>
@@ -1463,8 +1515,11 @@
       <c r="D13" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="14" spans="1:4">
+      <c r="E13" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
       <c r="A14" t="s">
         <v>4</v>
       </c>
@@ -1477,8 +1532,11 @@
       <c r="D14" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="15" spans="1:4">
+      <c r="E14" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
       <c r="A15" t="s">
         <v>4</v>
       </c>
@@ -1491,8 +1549,11 @@
       <c r="D15" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="16" spans="1:4">
+      <c r="E15" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
       <c r="A16" t="s">
         <v>4</v>
       </c>
@@ -1505,8 +1566,11 @@
       <c r="D16" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="17" spans="1:4">
+      <c r="E16" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
       <c r="A17" t="s">
         <v>4</v>
       </c>
@@ -1519,8 +1583,11 @@
       <c r="D17" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="18" spans="1:4">
+      <c r="E17" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
       <c r="A18" t="s">
         <v>4</v>
       </c>
@@ -1533,8 +1600,11 @@
       <c r="D18" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="19" spans="1:4">
+      <c r="E18" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
       <c r="A19" t="s">
         <v>4</v>
       </c>
@@ -1547,8 +1617,11 @@
       <c r="D19" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="20" spans="1:4">
+      <c r="E19" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
       <c r="A20" t="s">
         <v>4</v>
       </c>
@@ -1561,8 +1634,11 @@
       <c r="D20" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="21" spans="1:4">
+      <c r="E20" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
       <c r="A21" t="s">
         <v>4</v>
       </c>
@@ -1573,6 +1649,9 @@
         <v>0.4</v>
       </c>
       <c r="D21" t="s">
+        <v>37</v>
+      </c>
+      <c r="E21" t="s">
         <v>37</v>
       </c>
     </row>
@@ -1583,19 +1662,20 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4954F1F7-25CD-4C45-BDC1-E6036E057A74}">
-  <dimension ref="A1:D22"/>
+  <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="M14" sqref="M14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="2" max="2" width="16.83203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="20.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1608,8 +1688,11 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4">
+      <c r="E1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -1619,8 +1702,11 @@
       <c r="D2" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="3" spans="1:4">
+      <c r="E2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -1633,8 +1719,11 @@
       <c r="D3" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="4" spans="1:4">
+      <c r="E3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -1644,8 +1733,11 @@
       <c r="D4" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="5" spans="1:4">
+      <c r="E4" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -1655,8 +1747,11 @@
       <c r="D5" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="6" spans="1:4">
+      <c r="E5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -1666,8 +1761,11 @@
       <c r="D6" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="7" spans="1:4">
+      <c r="E6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -1680,8 +1778,11 @@
       <c r="D7" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="8" spans="1:4">
+      <c r="E7" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
       <c r="A8" t="s">
         <v>4</v>
       </c>
@@ -1691,8 +1792,11 @@
       <c r="D8" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="9" spans="1:4">
+      <c r="E8" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
       <c r="A9" t="s">
         <v>4</v>
       </c>
@@ -1702,8 +1806,11 @@
       <c r="D9" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="10" spans="1:4">
+      <c r="E9" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
       <c r="A10" t="s">
         <v>4</v>
       </c>
@@ -1713,8 +1820,11 @@
       <c r="D10" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="11" spans="1:4">
+      <c r="E10" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
       <c r="A11" t="s">
         <v>4</v>
       </c>
@@ -1724,8 +1834,11 @@
       <c r="D11" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="12" spans="1:4">
+      <c r="E11" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
       <c r="A12" t="s">
         <v>4</v>
       </c>
@@ -1735,8 +1848,11 @@
       <c r="D12" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="13" spans="1:4">
+      <c r="E12" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
       <c r="A13" t="s">
         <v>4</v>
       </c>
@@ -1749,8 +1865,11 @@
       <c r="D13" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="14" spans="1:4">
+      <c r="E13" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
       <c r="A14" t="s">
         <v>4</v>
       </c>
@@ -1763,8 +1882,11 @@
       <c r="D14" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="15" spans="1:4">
+      <c r="E14" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
       <c r="A15" t="s">
         <v>4</v>
       </c>
@@ -1774,8 +1896,11 @@
       <c r="D15" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="16" spans="1:4">
+      <c r="E15" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
       <c r="A16" t="s">
         <v>4</v>
       </c>
@@ -1788,8 +1913,11 @@
       <c r="D16" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="17" spans="1:4">
+      <c r="E16" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
       <c r="A17" t="s">
         <v>4</v>
       </c>
@@ -1799,8 +1927,11 @@
       <c r="D17" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="18" spans="1:4">
+      <c r="E17" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
       <c r="A18" t="s">
         <v>4</v>
       </c>
@@ -1813,8 +1944,11 @@
       <c r="D18" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="19" spans="1:4">
+      <c r="E18" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
       <c r="A19" t="s">
         <v>4</v>
       </c>
@@ -1824,8 +1958,11 @@
       <c r="D19" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="20" spans="1:4">
+      <c r="E19" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
       <c r="A20" t="s">
         <v>4</v>
       </c>
@@ -1838,8 +1975,11 @@
       <c r="D20" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="21" spans="1:4">
+      <c r="E20" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
       <c r="A21" t="s">
         <v>4</v>
       </c>
@@ -1849,8 +1989,11 @@
       <c r="D21" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="22" spans="1:4">
+      <c r="E21" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
       <c r="A22" t="s">
         <v>4</v>
       </c>
@@ -1861,6 +2004,9 @@
         <v>17</v>
       </c>
       <c r="D22" t="s">
+        <v>38</v>
+      </c>
+      <c r="E22" t="s">
         <v>38</v>
       </c>
     </row>

</xml_diff>

<commit_message>
overlaid terrestrial spp with crops!
</commit_message>
<xml_diff>
--- a/prep/02_feed/diet_composition_wrangling/salmon_aquaculture_diet_composition.xlsx
+++ b/prep/02_feed/diet_composition_wrangling/salmon_aquaculture_diet_composition.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gclawson/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{0C76173D-A066-5F46-9206-225135214F80}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{AD51801D-0648-8140-AAA3-EB5AA52F96C2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-33600" yWindow="1300" windowWidth="27640" windowHeight="16940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5500" yWindow="500" windowWidth="27640" windowHeight="16940" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2016" sheetId="1" r:id="rId1"/>
@@ -1001,7 +1001,7 @@
 <worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
@@ -1285,10 +1285,403 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:E21"/>
+  <dimension ref="A1:G21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="G16" sqref="G16:G19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <cols>
+    <col min="2" max="2" width="16.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2">
+        <v>20.9</v>
+      </c>
+      <c r="D2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3">
+        <v>9.8000000000000007</v>
+      </c>
+      <c r="D3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4">
+        <v>4.3</v>
+      </c>
+      <c r="D4" t="s">
+        <v>25</v>
+      </c>
+      <c r="E4" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5">
+        <v>3.4</v>
+      </c>
+      <c r="D5" t="s">
+        <v>26</v>
+      </c>
+      <c r="E5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6">
+        <v>1.4</v>
+      </c>
+      <c r="D6" t="s">
+        <v>27</v>
+      </c>
+      <c r="E6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7">
+        <v>0.7</v>
+      </c>
+      <c r="D7" t="s">
+        <v>8</v>
+      </c>
+      <c r="E7" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8">
+        <v>18</v>
+      </c>
+      <c r="D8" t="s">
+        <v>28</v>
+      </c>
+      <c r="E8" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9" t="s">
+        <v>4</v>
+      </c>
+      <c r="B9" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9">
+        <v>1.3</v>
+      </c>
+      <c r="D9" t="s">
+        <v>15</v>
+      </c>
+      <c r="E9" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10" t="s">
+        <v>4</v>
+      </c>
+      <c r="B10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C10">
+        <v>0.4</v>
+      </c>
+      <c r="D10" t="s">
+        <v>29</v>
+      </c>
+      <c r="E10" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="A11" t="s">
+        <v>4</v>
+      </c>
+      <c r="B11" t="s">
+        <v>5</v>
+      </c>
+      <c r="C11">
+        <v>0.4</v>
+      </c>
+      <c r="D11" t="s">
+        <v>30</v>
+      </c>
+      <c r="E11" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="A12" t="s">
+        <v>4</v>
+      </c>
+      <c r="B12" t="s">
+        <v>5</v>
+      </c>
+      <c r="C12">
+        <v>0.1</v>
+      </c>
+      <c r="D12" t="s">
+        <v>31</v>
+      </c>
+      <c r="E12" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="A13" t="s">
+        <v>4</v>
+      </c>
+      <c r="B13" t="s">
+        <v>5</v>
+      </c>
+      <c r="C13">
+        <v>6.5</v>
+      </c>
+      <c r="D13" t="s">
+        <v>16</v>
+      </c>
+      <c r="E13" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="A14" t="s">
+        <v>4</v>
+      </c>
+      <c r="B14" t="s">
+        <v>5</v>
+      </c>
+      <c r="C14">
+        <v>3.6</v>
+      </c>
+      <c r="D14" t="s">
+        <v>9</v>
+      </c>
+      <c r="E14" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
+      <c r="A15" t="s">
+        <v>4</v>
+      </c>
+      <c r="B15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C15">
+        <v>2.5</v>
+      </c>
+      <c r="D15" t="s">
+        <v>32</v>
+      </c>
+      <c r="E15" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7">
+      <c r="A16" t="s">
+        <v>4</v>
+      </c>
+      <c r="B16" t="s">
+        <v>5</v>
+      </c>
+      <c r="C16">
+        <v>8.8000000000000007</v>
+      </c>
+      <c r="D16" t="s">
+        <v>33</v>
+      </c>
+      <c r="E16" t="s">
+        <v>33</v>
+      </c>
+      <c r="G16">
+        <f>C16/(SUM($C$16:$C$19))</f>
+        <v>0.39285714285714285</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7">
+      <c r="A17" t="s">
+        <v>4</v>
+      </c>
+      <c r="B17" t="s">
+        <v>5</v>
+      </c>
+      <c r="C17">
+        <v>3.3</v>
+      </c>
+      <c r="D17" t="s">
+        <v>34</v>
+      </c>
+      <c r="E17" t="s">
+        <v>34</v>
+      </c>
+      <c r="G17">
+        <f t="shared" ref="G17:G19" si="0">C17/(SUM($C$16:$C$19))</f>
+        <v>0.14732142857142855</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7">
+      <c r="A18" t="s">
+        <v>4</v>
+      </c>
+      <c r="B18" t="s">
+        <v>5</v>
+      </c>
+      <c r="C18">
+        <v>8.3000000000000007</v>
+      </c>
+      <c r="D18" t="s">
+        <v>35</v>
+      </c>
+      <c r="E18" t="s">
+        <v>35</v>
+      </c>
+      <c r="G18">
+        <f t="shared" si="0"/>
+        <v>0.3705357142857143</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7">
+      <c r="A19" t="s">
+        <v>4</v>
+      </c>
+      <c r="B19" t="s">
+        <v>5</v>
+      </c>
+      <c r="C19">
+        <v>2</v>
+      </c>
+      <c r="D19" t="s">
+        <v>36</v>
+      </c>
+      <c r="E19" t="s">
+        <v>36</v>
+      </c>
+      <c r="G19">
+        <f t="shared" si="0"/>
+        <v>8.9285714285714274E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7">
+      <c r="A20" t="s">
+        <v>4</v>
+      </c>
+      <c r="B20" t="s">
+        <v>5</v>
+      </c>
+      <c r="C20">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="D20" t="s">
+        <v>23</v>
+      </c>
+      <c r="E20" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7">
+      <c r="A21" t="s">
+        <v>4</v>
+      </c>
+      <c r="B21" t="s">
+        <v>5</v>
+      </c>
+      <c r="C21">
+        <v>0.4</v>
+      </c>
+      <c r="D21" t="s">
+        <v>37</v>
+      </c>
+      <c r="E21" t="s">
+        <v>37</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4954F1F7-25CD-4C45-BDC1-E6036E057A74}">
+  <dimension ref="A1:E22"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1322,9 +1715,6 @@
       <c r="B2" t="s">
         <v>5</v>
       </c>
-      <c r="C2">
-        <v>20.9</v>
-      </c>
       <c r="D2" t="s">
         <v>24</v>
       </c>
@@ -1340,7 +1730,7 @@
         <v>5</v>
       </c>
       <c r="C3">
-        <v>9.8000000000000007</v>
+        <v>13</v>
       </c>
       <c r="D3" t="s">
         <v>7</v>
@@ -1356,9 +1746,6 @@
       <c r="B4" t="s">
         <v>5</v>
       </c>
-      <c r="C4">
-        <v>4.3</v>
-      </c>
       <c r="D4" t="s">
         <v>25</v>
       </c>
@@ -1373,9 +1760,6 @@
       <c r="B5" t="s">
         <v>5</v>
       </c>
-      <c r="C5">
-        <v>3.4</v>
-      </c>
       <c r="D5" t="s">
         <v>26</v>
       </c>
@@ -1390,9 +1774,6 @@
       <c r="B6" t="s">
         <v>5</v>
       </c>
-      <c r="C6">
-        <v>1.4</v>
-      </c>
       <c r="D6" t="s">
         <v>27</v>
       </c>
@@ -1408,7 +1789,7 @@
         <v>5</v>
       </c>
       <c r="C7">
-        <v>0.7</v>
+        <v>4</v>
       </c>
       <c r="D7" t="s">
         <v>8</v>
@@ -1424,9 +1805,6 @@
       <c r="B8" t="s">
         <v>5</v>
       </c>
-      <c r="C8">
-        <v>18</v>
-      </c>
       <c r="D8" t="s">
         <v>28</v>
       </c>
@@ -1441,9 +1819,6 @@
       <c r="B9" t="s">
         <v>5</v>
       </c>
-      <c r="C9">
-        <v>1.3</v>
-      </c>
       <c r="D9" t="s">
         <v>15</v>
       </c>
@@ -1458,9 +1833,6 @@
       <c r="B10" t="s">
         <v>5</v>
       </c>
-      <c r="C10">
-        <v>0.4</v>
-      </c>
       <c r="D10" t="s">
         <v>29</v>
       </c>
@@ -1475,9 +1847,6 @@
       <c r="B11" t="s">
         <v>5</v>
       </c>
-      <c r="C11">
-        <v>0.4</v>
-      </c>
       <c r="D11" t="s">
         <v>30</v>
       </c>
@@ -1492,9 +1861,6 @@
       <c r="B12" t="s">
         <v>5</v>
       </c>
-      <c r="C12">
-        <v>0.1</v>
-      </c>
       <c r="D12" t="s">
         <v>31</v>
       </c>
@@ -1510,7 +1876,7 @@
         <v>5</v>
       </c>
       <c r="C13">
-        <v>6.5</v>
+        <v>7</v>
       </c>
       <c r="D13" t="s">
         <v>16</v>
@@ -1527,7 +1893,7 @@
         <v>5</v>
       </c>
       <c r="C14">
-        <v>3.6</v>
+        <v>2</v>
       </c>
       <c r="D14" t="s">
         <v>9</v>
@@ -1543,9 +1909,6 @@
       <c r="B15" t="s">
         <v>5</v>
       </c>
-      <c r="C15">
-        <v>2.5</v>
-      </c>
       <c r="D15" t="s">
         <v>32</v>
       </c>
@@ -1561,7 +1924,7 @@
         <v>5</v>
       </c>
       <c r="C16">
-        <v>8.8000000000000007</v>
+        <v>21.607142857142858</v>
       </c>
       <c r="D16" t="s">
         <v>33</v>
@@ -1578,7 +1941,7 @@
         <v>5</v>
       </c>
       <c r="C17">
-        <v>3.3</v>
+        <v>8.1026785714285694</v>
       </c>
       <c r="D17" t="s">
         <v>34</v>
@@ -1595,7 +1958,7 @@
         <v>5</v>
       </c>
       <c r="C18">
-        <v>8.3000000000000007</v>
+        <v>20.379464285714288</v>
       </c>
       <c r="D18" t="s">
         <v>35</v>
@@ -1612,348 +1975,7 @@
         <v>5</v>
       </c>
       <c r="C19">
-        <v>2</v>
-      </c>
-      <c r="D19" t="s">
-        <v>36</v>
-      </c>
-      <c r="E19" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5">
-      <c r="A20" t="s">
-        <v>4</v>
-      </c>
-      <c r="B20" t="s">
-        <v>5</v>
-      </c>
-      <c r="C20">
-        <v>4.0999999999999996</v>
-      </c>
-      <c r="D20" t="s">
-        <v>23</v>
-      </c>
-      <c r="E20" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5">
-      <c r="A21" t="s">
-        <v>4</v>
-      </c>
-      <c r="B21" t="s">
-        <v>5</v>
-      </c>
-      <c r="C21">
-        <v>0.4</v>
-      </c>
-      <c r="D21" t="s">
-        <v>37</v>
-      </c>
-      <c r="E21" t="s">
-        <v>37</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4954F1F7-25CD-4C45-BDC1-E6036E057A74}">
-  <dimension ref="A1:E22"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
-  <cols>
-    <col min="2" max="2" width="16.83203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.1640625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5">
-      <c r="A2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" t="s">
-        <v>24</v>
-      </c>
-      <c r="E2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
-      <c r="A3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3">
-        <v>13</v>
-      </c>
-      <c r="D3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="A4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D4" t="s">
-        <v>25</v>
-      </c>
-      <c r="E4" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
-      <c r="A5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
-        <v>5</v>
-      </c>
-      <c r="D5" t="s">
-        <v>26</v>
-      </c>
-      <c r="E5" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5">
-      <c r="A6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6" t="s">
-        <v>5</v>
-      </c>
-      <c r="D6" t="s">
-        <v>27</v>
-      </c>
-      <c r="E6" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5">
-      <c r="A7" t="s">
-        <v>4</v>
-      </c>
-      <c r="B7" t="s">
-        <v>5</v>
-      </c>
-      <c r="C7">
-        <v>4</v>
-      </c>
-      <c r="D7" t="s">
-        <v>8</v>
-      </c>
-      <c r="E7" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5">
-      <c r="A8" t="s">
-        <v>4</v>
-      </c>
-      <c r="B8" t="s">
-        <v>5</v>
-      </c>
-      <c r="D8" t="s">
-        <v>28</v>
-      </c>
-      <c r="E8" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5">
-      <c r="A9" t="s">
-        <v>4</v>
-      </c>
-      <c r="B9" t="s">
-        <v>5</v>
-      </c>
-      <c r="D9" t="s">
-        <v>15</v>
-      </c>
-      <c r="E9" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5">
-      <c r="A10" t="s">
-        <v>4</v>
-      </c>
-      <c r="B10" t="s">
-        <v>5</v>
-      </c>
-      <c r="D10" t="s">
-        <v>29</v>
-      </c>
-      <c r="E10" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5">
-      <c r="A11" t="s">
-        <v>4</v>
-      </c>
-      <c r="B11" t="s">
-        <v>5</v>
-      </c>
-      <c r="D11" t="s">
-        <v>30</v>
-      </c>
-      <c r="E11" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5">
-      <c r="A12" t="s">
-        <v>4</v>
-      </c>
-      <c r="B12" t="s">
-        <v>5</v>
-      </c>
-      <c r="D12" t="s">
-        <v>31</v>
-      </c>
-      <c r="E12" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5">
-      <c r="A13" t="s">
-        <v>4</v>
-      </c>
-      <c r="B13" t="s">
-        <v>5</v>
-      </c>
-      <c r="C13">
-        <v>7</v>
-      </c>
-      <c r="D13" t="s">
-        <v>16</v>
-      </c>
-      <c r="E13" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5">
-      <c r="A14" t="s">
-        <v>4</v>
-      </c>
-      <c r="B14" t="s">
-        <v>5</v>
-      </c>
-      <c r="C14">
-        <v>2</v>
-      </c>
-      <c r="D14" t="s">
-        <v>9</v>
-      </c>
-      <c r="E14" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5">
-      <c r="A15" t="s">
-        <v>4</v>
-      </c>
-      <c r="B15" t="s">
-        <v>5</v>
-      </c>
-      <c r="D15" t="s">
-        <v>32</v>
-      </c>
-      <c r="E15" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5">
-      <c r="A16" t="s">
-        <v>4</v>
-      </c>
-      <c r="B16" t="s">
-        <v>5</v>
-      </c>
-      <c r="C16">
-        <v>32</v>
-      </c>
-      <c r="D16" t="s">
-        <v>33</v>
-      </c>
-      <c r="E16" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5">
-      <c r="A17" t="s">
-        <v>4</v>
-      </c>
-      <c r="B17" t="s">
-        <v>5</v>
-      </c>
-      <c r="D17" t="s">
-        <v>34</v>
-      </c>
-      <c r="E17" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5">
-      <c r="A18" t="s">
-        <v>4</v>
-      </c>
-      <c r="B18" t="s">
-        <v>5</v>
-      </c>
-      <c r="C18">
-        <v>23</v>
-      </c>
-      <c r="D18" t="s">
-        <v>35</v>
-      </c>
-      <c r="E18" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5">
-      <c r="A19" t="s">
-        <v>4</v>
-      </c>
-      <c r="B19" t="s">
-        <v>5</v>
+        <v>4.9107142857142847</v>
       </c>
       <c r="D19" t="s">
         <v>36</v>

</xml_diff>